<commit_message>
Shared data added til labeled data in ASKE-label
</commit_message>
<xml_diff>
--- a/data/labeled_data/Aske.xlsx
+++ b/data/labeled_data/Aske.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD0EB69-8ECB-4D82-BBD0-CB00F7DB2476}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377E5B25-A6BF-4BD5-A2FD-A86543B232E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2263" yWindow="2263" windowWidth="17588" windowHeight="10988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unique" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="331">
   <si>
     <t xml:space="preserve">The same whale spiked up btc decides to drop the hammer.. there will be chaos_x000D_
 </t>
@@ -1683,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B251"/>
+  <dimension ref="A1:B325"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
+      <selection activeCell="A223" sqref="A223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1695,8 +1695,8 @@
     <col min="2" max="2" width="25.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
         <v>319</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -3495,83 +3495,805 @@
         <v>324</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B226" s="1"/>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B227" s="1"/>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B228" s="1"/>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B229" s="1"/>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B230" s="1"/>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B231" s="1"/>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B232" s="1"/>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B233" s="1"/>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B234" s="1"/>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B235" s="1"/>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B236" s="1"/>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B237" s="1"/>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B238" s="1"/>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B239" s="1"/>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B240" s="1"/>
-    </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B241" s="1"/>
-    </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B242" s="1"/>
-    </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B243" s="1"/>
-    </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B244" s="1"/>
-    </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B245" s="1"/>
-    </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B246" s="1"/>
-    </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B247" s="1"/>
-    </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B248" s="1"/>
-    </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B249" s="1"/>
-    </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B250" s="1"/>
-    </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B251" s="1"/>
+    <row r="226" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A226" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B226" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A227" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B227" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A228" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B228" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A229" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B229" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A230" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B230" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A231" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B231" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A232" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B232" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A233" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B233" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A234" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B234" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A235" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B235" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A236" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B236" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A237" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B237" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A238" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B238" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A239" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B239" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A240" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B240" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A241" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B241" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A242" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B242" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A243" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B243" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A244" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B244" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A245" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B245" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A246" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B246" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A247" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B247" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A248" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B248" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A249" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B249" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A250" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B250" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A251" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B251" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A252" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B252" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A253" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B253" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A254" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B254" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A255" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B255" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A256" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B256" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A257" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B257" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A258" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B258" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A259" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B259" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A260" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B260" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A261" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B261" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A262" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B262" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A263" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B263" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A264" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B264" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A265" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B265" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A266" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B266" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A267" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B267" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A268" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B268" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A269" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B269" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A270" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B270" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A271" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B271" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A272" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B272" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A273" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B273" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A274" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B274" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A275" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B275" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A276" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B276" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A277" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B277" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A278" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B278" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A279" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B279" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A280" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B280" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A281" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B281" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A282" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B282" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A283" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B283" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A284" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B284" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A285" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B285" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A286" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B286" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A287" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B287" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A288" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B288" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A289" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B289" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A290" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B290" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A291" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B291" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A292" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B292" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A293" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B293" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A294" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B294" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A295" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B295" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A296" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B296" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A297" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B297" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A298" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B298" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A299" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B299" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A300" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B300" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A301" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B301" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A302" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B302" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A303" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B303" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A304" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B304" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A305" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B305" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A306" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B306" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A307" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B307" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A308" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B308" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A309" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B309" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A310" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B310" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A311" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B311" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A312" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B312" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A313" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B313" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A314" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B314" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A315" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B315" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A316" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B316" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A317" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B317" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A318" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B318" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A319" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B319" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A320" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B320" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="A321" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B321" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A322" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B322" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A323" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B323" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A324" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B324" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A325" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B325" t="s">
+        <v>324</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B225" xr:uid="{86323A8B-8F21-4CE6-B9D2-7214EF8112BD}"/>
@@ -3585,6 +4307,7 @@
     <hyperlink ref="A83" r:id="rId7" xr:uid="{60F4CE60-6E4C-4653-B503-3A914AF1B8C0}"/>
     <hyperlink ref="A54" r:id="rId8" xr:uid="{BD51A9C2-3AB7-4F3E-B5B2-E65B65DC7948}"/>
     <hyperlink ref="A12" r:id="rId9" xr:uid="{F8E71DB4-7C74-4678-B1AF-4135634708CC}"/>
+    <hyperlink ref="A285" r:id="rId10" xr:uid="{DEC0E613-E448-4EE0-B5E6-00EBCA77BD39}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3592,11 +4315,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A895C986-5639-41B7-97E4-8502EF320921}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3616,7 +4338,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3627,7 +4349,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3638,7 +4360,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="72.900000000000006" hidden="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3649,7 +4371,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3660,7 +4382,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3671,7 +4393,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3682,7 +4404,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3704,7 +4426,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3726,7 +4448,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3748,7 +4470,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="58.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3759,7 +4481,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3770,7 +4492,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3792,7 +4514,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="58.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3814,7 +4536,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3825,7 +4547,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3847,7 +4569,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3858,7 +4580,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3869,7 +4591,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3880,7 +4602,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3891,7 +4613,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3902,7 +4624,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3913,7 +4635,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3935,7 +4657,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="58.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3946,7 +4668,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3957,7 +4679,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3968,7 +4690,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3979,7 +4701,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3990,7 +4712,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4001,7 +4723,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4012,7 +4734,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4023,7 +4745,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4045,7 +4767,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="72.900000000000006" hidden="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4067,7 +4789,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4078,7 +4800,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4089,7 +4811,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4100,7 +4822,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4111,7 +4833,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="58.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4122,7 +4844,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="72.900000000000006" hidden="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4144,7 +4866,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4155,7 +4877,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4166,7 +4888,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4177,7 +4899,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4188,7 +4910,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4199,7 +4921,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4232,7 +4954,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4265,7 +4987,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4276,7 +4998,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4287,7 +5009,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4298,7 +5020,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4309,7 +5031,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4320,7 +5042,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="58.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4331,7 +5053,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4353,7 +5075,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4364,7 +5086,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4375,7 +5097,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4397,7 +5119,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4408,7 +5130,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4419,7 +5141,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="58.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4430,7 +5152,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4441,7 +5163,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4463,7 +5185,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4474,7 +5196,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4485,7 +5207,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4496,7 +5218,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4518,7 +5240,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4529,7 +5251,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4540,7 +5262,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4551,7 +5273,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4573,7 +5295,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4584,7 +5306,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4595,7 +5317,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4606,7 +5328,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4628,7 +5350,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="43.75" hidden="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:3" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4639,7 +5361,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="58.3" hidden="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:3" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4650,7 +5372,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4661,7 +5383,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="87.45" hidden="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:3" ht="87.45" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4672,7 +5394,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="29.15" hidden="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:3" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4694,7 +5416,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="72.900000000000006" hidden="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:3" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4717,13 +5439,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C101" xr:uid="{C4586E1C-8DF8-45A6-A9EA-CE13802A414A}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="POS"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C101" xr:uid="{C4586E1C-8DF8-45A6-A9EA-CE13802A414A}"/>
   <hyperlinks>
     <hyperlink ref="B61" r:id="rId1" xr:uid="{D5864DC2-6911-4832-85F0-7E97A621681A}"/>
   </hyperlinks>

</xml_diff>